<commit_message>
Añadiendo nuevos archivos - DOCUMENTACIÓN
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/DIAGRAMA DE GANTT/GANTT_CoolSound.xlsx
+++ b/DOCUMENTACION/DIAGRAMA DE GANTT/GANTT_CoolSound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raban\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E96BD2-F766-4DE3-A8A7-042FADCAF351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1769FA-9A49-419B-AEBC-09F2144AE0AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
   <si>
     <t>TITULO PROYECTO</t>
   </si>
@@ -131,15 +131,6 @@
   </si>
   <si>
     <t>SEMANA 18</t>
-  </si>
-  <si>
-    <t>SEMANA 19</t>
-  </si>
-  <si>
-    <t>SEMANA 20</t>
-  </si>
-  <si>
-    <t>SEMANA 21</t>
   </si>
   <si>
     <t>L</t>
@@ -370,7 +361,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,8 +536,62 @@
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF525252"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFEDEDED"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFDBDBDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -708,11 +753,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -793,82 +923,140 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="29" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="29" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="30" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="30" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1310,7 +1498,7 @@
   <dimension ref="A1:EC29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT30" sqref="AT30"/>
+      <selection activeCell="DA19" sqref="DA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1397,14 +1585,14 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1422,15 +1610,15 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
+      <c r="AF2" s="46"/>
+      <c r="AG2" s="46"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
@@ -1537,46 +1725,46 @@
       <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="D4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="57" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="49"/>
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AF4" s="49"/>
+      <c r="AG4" s="49"/>
+      <c r="AH4" s="49"/>
+      <c r="AI4" s="49"/>
+      <c r="AJ4" s="49"/>
+      <c r="AK4" s="49"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
@@ -1614,46 +1802,46 @@
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52" t="s">
+      <c r="D5" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="60">
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="52">
         <v>44098</v>
       </c>
-      <c r="R5" s="61"/>
-      <c r="S5" s="61"/>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="58"/>
-      <c r="Y5" s="58"/>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58"/>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58"/>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58"/>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="59"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AI5" s="38"/>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="39"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
@@ -1762,617 +1950,579 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="54" t="s">
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="54"/>
-      <c r="AC7" s="54"/>
-      <c r="AD7" s="54"/>
-      <c r="AE7" s="54"/>
-      <c r="AF7" s="54"/>
-      <c r="AG7" s="54"/>
-      <c r="AH7" s="54"/>
-      <c r="AI7" s="54"/>
-      <c r="AJ7" s="54"/>
-      <c r="AK7" s="54"/>
-      <c r="AL7" s="48" t="s">
+      <c r="X7" s="51"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="51"/>
+      <c r="AB7" s="51"/>
+      <c r="AC7" s="51"/>
+      <c r="AD7" s="51"/>
+      <c r="AE7" s="51"/>
+      <c r="AF7" s="51"/>
+      <c r="AG7" s="51"/>
+      <c r="AH7" s="51"/>
+      <c r="AI7" s="51"/>
+      <c r="AJ7" s="51"/>
+      <c r="AK7" s="51"/>
+      <c r="AL7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="AM7" s="48"/>
-      <c r="AN7" s="48"/>
-      <c r="AO7" s="48"/>
-      <c r="AP7" s="48"/>
-      <c r="AQ7" s="48"/>
-      <c r="AR7" s="48"/>
-      <c r="AS7" s="48"/>
-      <c r="AT7" s="48"/>
-      <c r="AU7" s="48"/>
-      <c r="AV7" s="48"/>
-      <c r="AW7" s="48"/>
-      <c r="AX7" s="48"/>
-      <c r="AY7" s="48"/>
-      <c r="AZ7" s="48"/>
-      <c r="BA7" s="49" t="s">
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="54"/>
+      <c r="AO7" s="54"/>
+      <c r="AP7" s="54"/>
+      <c r="AQ7" s="54"/>
+      <c r="AR7" s="54"/>
+      <c r="AS7" s="54"/>
+      <c r="AT7" s="54"/>
+      <c r="AU7" s="54"/>
+      <c r="AV7" s="54"/>
+      <c r="AW7" s="54"/>
+      <c r="AX7" s="54"/>
+      <c r="AY7" s="54"/>
+      <c r="AZ7" s="54"/>
+      <c r="BA7" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="BB7" s="49"/>
-      <c r="BC7" s="49"/>
-      <c r="BD7" s="49"/>
-      <c r="BE7" s="49"/>
-      <c r="BF7" s="49"/>
-      <c r="BG7" s="49"/>
-      <c r="BH7" s="49"/>
-      <c r="BI7" s="49"/>
-      <c r="BJ7" s="49"/>
-      <c r="BK7" s="49"/>
-      <c r="BL7" s="49"/>
-      <c r="BM7" s="49"/>
-      <c r="BN7" s="49"/>
-      <c r="BO7" s="49"/>
-      <c r="BP7" s="50" t="s">
+      <c r="BB7" s="55"/>
+      <c r="BC7" s="55"/>
+      <c r="BD7" s="55"/>
+      <c r="BE7" s="55"/>
+      <c r="BF7" s="55"/>
+      <c r="BG7" s="55"/>
+      <c r="BH7" s="55"/>
+      <c r="BI7" s="55"/>
+      <c r="BJ7" s="55"/>
+      <c r="BK7" s="55"/>
+      <c r="BL7" s="55"/>
+      <c r="BM7" s="55"/>
+      <c r="BN7" s="55"/>
+      <c r="BO7" s="55"/>
+      <c r="BP7" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="BQ7" s="50"/>
-      <c r="BR7" s="50"/>
-      <c r="BS7" s="50"/>
-      <c r="BT7" s="50"/>
-      <c r="BU7" s="50"/>
-      <c r="BV7" s="50"/>
-      <c r="BW7" s="50"/>
-      <c r="BX7" s="50"/>
-      <c r="BY7" s="50"/>
-      <c r="BZ7" s="50"/>
-      <c r="CA7" s="50"/>
-      <c r="CB7" s="50"/>
-      <c r="CC7" s="50"/>
-      <c r="CD7" s="50"/>
-      <c r="CE7" s="50" t="s">
+      <c r="BQ7" s="56"/>
+      <c r="BR7" s="56"/>
+      <c r="BS7" s="56"/>
+      <c r="BT7" s="56"/>
+      <c r="BU7" s="56"/>
+      <c r="BV7" s="56"/>
+      <c r="BW7" s="56"/>
+      <c r="BX7" s="56"/>
+      <c r="BY7" s="56"/>
+      <c r="BZ7" s="56"/>
+      <c r="CA7" s="56"/>
+      <c r="CB7" s="56"/>
+      <c r="CC7" s="56"/>
+      <c r="CD7" s="56"/>
+      <c r="CE7" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="CF7" s="50"/>
-      <c r="CG7" s="50"/>
-      <c r="CH7" s="50"/>
-      <c r="CI7" s="50"/>
-      <c r="CJ7" s="50"/>
-      <c r="CK7" s="50"/>
-      <c r="CL7" s="50"/>
-      <c r="CM7" s="50"/>
-      <c r="CN7" s="50"/>
-      <c r="CO7" s="50"/>
-      <c r="CP7" s="50"/>
-      <c r="CQ7" s="50"/>
-      <c r="CR7" s="50"/>
-      <c r="CS7" s="50"/>
-      <c r="CT7" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="CU7" s="50"/>
-      <c r="CV7" s="50"/>
-      <c r="CW7" s="50"/>
-      <c r="CX7" s="50"/>
-      <c r="CY7" s="50"/>
-      <c r="CZ7" s="50"/>
-      <c r="DA7" s="50"/>
-      <c r="DB7" s="50"/>
-      <c r="DC7" s="50"/>
-      <c r="DD7" s="50"/>
-      <c r="DE7" s="50"/>
-      <c r="DF7" s="50"/>
-      <c r="DG7" s="50"/>
-      <c r="DH7" s="50"/>
+      <c r="CF7" s="74"/>
+      <c r="CG7" s="74"/>
+      <c r="CH7" s="74"/>
+      <c r="CI7" s="74"/>
+      <c r="CJ7" s="74"/>
+      <c r="CK7" s="74"/>
+      <c r="CL7" s="74"/>
+      <c r="CM7" s="74"/>
+      <c r="CN7" s="74"/>
+      <c r="CO7" s="74"/>
+      <c r="CP7" s="74"/>
+      <c r="CQ7" s="74"/>
+      <c r="CR7" s="74"/>
+      <c r="CS7" s="75"/>
+      <c r="CT7" s="69"/>
+      <c r="CU7" s="69"/>
+      <c r="CV7" s="69"/>
+      <c r="CW7" s="69"/>
+      <c r="CX7" s="69"/>
+      <c r="CY7" s="69"/>
+      <c r="CZ7" s="69"/>
+      <c r="DA7" s="69"/>
+      <c r="DB7" s="69"/>
+      <c r="DC7" s="69"/>
+      <c r="DD7" s="69"/>
+      <c r="DE7" s="69"/>
+      <c r="DF7" s="69"/>
+      <c r="DG7" s="69"/>
+      <c r="DH7" s="69"/>
     </row>
     <row r="8" spans="1:112" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45" t="s">
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45" t="s">
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="41" t="s">
+      <c r="S8" s="61"/>
+      <c r="T8" s="61"/>
+      <c r="U8" s="61"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41" t="s">
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="41"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
-      <c r="AG8" s="41" t="s">
+      <c r="AC8" s="62"/>
+      <c r="AD8" s="62"/>
+      <c r="AE8" s="62"/>
+      <c r="AF8" s="62"/>
+      <c r="AG8" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="AH8" s="41"/>
-      <c r="AI8" s="41"/>
-      <c r="AJ8" s="41"/>
-      <c r="AK8" s="41"/>
-      <c r="AL8" s="42" t="s">
+      <c r="AH8" s="62"/>
+      <c r="AI8" s="62"/>
+      <c r="AJ8" s="62"/>
+      <c r="AK8" s="62"/>
+      <c r="AL8" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="AM8" s="42"/>
-      <c r="AN8" s="42"/>
-      <c r="AO8" s="42"/>
-      <c r="AP8" s="42"/>
-      <c r="AQ8" s="43" t="s">
+      <c r="AM8" s="66"/>
+      <c r="AN8" s="66"/>
+      <c r="AO8" s="66"/>
+      <c r="AP8" s="66"/>
+      <c r="AQ8" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="AR8" s="43"/>
-      <c r="AS8" s="43"/>
-      <c r="AT8" s="43"/>
-      <c r="AU8" s="43"/>
-      <c r="AV8" s="43" t="s">
+      <c r="AR8" s="59"/>
+      <c r="AS8" s="59"/>
+      <c r="AT8" s="59"/>
+      <c r="AU8" s="59"/>
+      <c r="AV8" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="AW8" s="43"/>
-      <c r="AX8" s="43"/>
-      <c r="AY8" s="43"/>
-      <c r="AZ8" s="43"/>
-      <c r="BA8" s="40" t="s">
+      <c r="AW8" s="59"/>
+      <c r="AX8" s="59"/>
+      <c r="AY8" s="59"/>
+      <c r="AZ8" s="59"/>
+      <c r="BA8" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="BB8" s="40"/>
-      <c r="BC8" s="40"/>
-      <c r="BD8" s="40"/>
-      <c r="BE8" s="40"/>
-      <c r="BF8" s="40" t="s">
+      <c r="BB8" s="65"/>
+      <c r="BC8" s="65"/>
+      <c r="BD8" s="65"/>
+      <c r="BE8" s="65"/>
+      <c r="BF8" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="BG8" s="40"/>
-      <c r="BH8" s="40"/>
-      <c r="BI8" s="40"/>
-      <c r="BJ8" s="40"/>
-      <c r="BK8" s="40" t="s">
+      <c r="BG8" s="65"/>
+      <c r="BH8" s="65"/>
+      <c r="BI8" s="65"/>
+      <c r="BJ8" s="65"/>
+      <c r="BK8" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="BL8" s="40"/>
-      <c r="BM8" s="40"/>
-      <c r="BN8" s="40"/>
-      <c r="BO8" s="40"/>
-      <c r="BP8" s="38" t="s">
+      <c r="BL8" s="65"/>
+      <c r="BM8" s="65"/>
+      <c r="BN8" s="65"/>
+      <c r="BO8" s="65"/>
+      <c r="BP8" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="BQ8" s="38"/>
-      <c r="BR8" s="38"/>
-      <c r="BS8" s="38"/>
-      <c r="BT8" s="38"/>
-      <c r="BU8" s="38" t="s">
+      <c r="BQ8" s="63"/>
+      <c r="BR8" s="63"/>
+      <c r="BS8" s="63"/>
+      <c r="BT8" s="63"/>
+      <c r="BU8" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="BV8" s="38"/>
-      <c r="BW8" s="38"/>
-      <c r="BX8" s="38"/>
-      <c r="BY8" s="38"/>
-      <c r="BZ8" s="38" t="s">
+      <c r="BV8" s="63"/>
+      <c r="BW8" s="63"/>
+      <c r="BX8" s="63"/>
+      <c r="BY8" s="63"/>
+      <c r="BZ8" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="CA8" s="38"/>
-      <c r="CB8" s="38"/>
-      <c r="CC8" s="38"/>
-      <c r="CD8" s="38"/>
-      <c r="CE8" s="38" t="s">
+      <c r="CA8" s="63"/>
+      <c r="CB8" s="63"/>
+      <c r="CC8" s="63"/>
+      <c r="CD8" s="63"/>
+      <c r="CE8" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="CF8" s="38"/>
-      <c r="CG8" s="38"/>
-      <c r="CH8" s="38"/>
-      <c r="CI8" s="38"/>
-      <c r="CJ8" s="38" t="s">
+      <c r="CF8" s="63"/>
+      <c r="CG8" s="63"/>
+      <c r="CH8" s="63"/>
+      <c r="CI8" s="63"/>
+      <c r="CJ8" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="CK8" s="38"/>
-      <c r="CL8" s="38"/>
-      <c r="CM8" s="38"/>
-      <c r="CN8" s="38"/>
-      <c r="CO8" s="38" t="s">
+      <c r="CK8" s="63"/>
+      <c r="CL8" s="63"/>
+      <c r="CM8" s="63"/>
+      <c r="CN8" s="63"/>
+      <c r="CO8" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="CP8" s="38"/>
-      <c r="CQ8" s="38"/>
-      <c r="CR8" s="38"/>
-      <c r="CS8" s="38"/>
-      <c r="CT8" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="CU8" s="38"/>
-      <c r="CV8" s="38"/>
-      <c r="CW8" s="38"/>
-      <c r="CX8" s="38"/>
-      <c r="CY8" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ8" s="38"/>
-      <c r="DA8" s="38"/>
-      <c r="DB8" s="38"/>
-      <c r="DC8" s="38"/>
-      <c r="DD8" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="DE8" s="38"/>
-      <c r="DF8" s="38"/>
-      <c r="DG8" s="38"/>
-      <c r="DH8" s="38"/>
+      <c r="CP8" s="63"/>
+      <c r="CQ8" s="63"/>
+      <c r="CR8" s="63"/>
+      <c r="CS8" s="78"/>
+      <c r="CT8" s="69"/>
+      <c r="CU8" s="69"/>
+      <c r="CV8" s="69"/>
+      <c r="CW8" s="69"/>
+      <c r="CX8" s="69"/>
+      <c r="CY8" s="72"/>
+      <c r="CZ8" s="70"/>
+      <c r="DA8" s="70"/>
+      <c r="DB8" s="70"/>
+      <c r="DC8" s="71"/>
+      <c r="DD8" s="69"/>
+      <c r="DE8" s="69"/>
+      <c r="DF8" s="69"/>
+      <c r="DG8" s="69"/>
+      <c r="DH8" s="69"/>
     </row>
     <row r="9" spans="1:112" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="44"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="M9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="Q9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="R9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="V9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="T9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="V9" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="W9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="X9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="X9" s="11" t="s">
+      <c r="AA9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Y9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA9" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="AB9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AC9" s="11" t="s">
+      <c r="AF9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AD9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF9" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="AG9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AH9" s="11" t="s">
+      <c r="AK9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AI9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK9" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="AL9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AM9" s="12" t="s">
+      <c r="AP9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AN9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP9" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="AQ9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AR9" s="12" t="s">
+      <c r="AU9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AS9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU9" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="AV9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AW9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AW9" s="12" t="s">
+      <c r="AZ9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AX9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AY9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AZ9" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="BA9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="BB9" s="13" t="s">
+      <c r="BE9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="BC9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="BE9" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="BF9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="BG9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="BG9" s="13" t="s">
+      <c r="BJ9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="BH9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="BI9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="BJ9" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="BK9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="BL9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="BM9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="BN9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="BL9" s="13" t="s">
+      <c r="BO9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="BN9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="BO9" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="BP9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BQ9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="BS9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="BQ9" s="14" t="s">
+      <c r="BT9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="BR9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BS9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="BT9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="BU9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BV9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="BX9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="BV9" s="14" t="s">
+      <c r="BY9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="BW9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BX9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="BY9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="BZ9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="CA9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="CC9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="CA9" s="14" t="s">
+      <c r="CD9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="CB9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="CC9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="CD9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="CE9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="CF9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="CH9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="CF9" s="14" t="s">
+      <c r="CI9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="CG9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="CH9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="CI9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="CJ9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="CK9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="CM9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="CK9" s="14" t="s">
+      <c r="CN9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="CL9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="CM9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="CN9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="CO9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="CP9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="CR9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="CP9" s="14" t="s">
+      <c r="CS9" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="CQ9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="CR9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="CS9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="CT9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="CU9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="CV9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="CW9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="CX9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="CY9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="CZ9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="DA9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="DB9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="DC9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="DD9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="DE9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="DF9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="DG9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="DH9" s="14" t="s">
-        <v>42</v>
-      </c>
+      <c r="CT9" s="68"/>
+      <c r="CU9" s="68"/>
+      <c r="CV9" s="68"/>
+      <c r="CW9" s="68"/>
+      <c r="CX9" s="68"/>
+      <c r="CY9" s="68"/>
+      <c r="CZ9" s="68"/>
+      <c r="DA9" s="68"/>
+      <c r="DB9" s="68"/>
+      <c r="DC9" s="68"/>
+      <c r="DD9" s="68"/>
+      <c r="DE9" s="68"/>
+      <c r="DF9" s="68"/>
+      <c r="DG9" s="68"/>
+      <c r="DH9" s="68"/>
     </row>
     <row r="10" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2380,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -2475,30 +2625,30 @@
       <c r="CP10" s="20"/>
       <c r="CQ10" s="20"/>
       <c r="CR10" s="20"/>
-      <c r="CS10" s="20"/>
-      <c r="CT10" s="20"/>
-      <c r="CU10" s="20"/>
-      <c r="CV10" s="20"/>
-      <c r="CW10" s="20"/>
-      <c r="CX10" s="20"/>
-      <c r="CY10" s="20"/>
-      <c r="CZ10" s="20"/>
-      <c r="DA10" s="20"/>
-      <c r="DB10" s="20"/>
-      <c r="DC10" s="20"/>
-      <c r="DD10" s="20"/>
-      <c r="DE10" s="20"/>
-      <c r="DF10" s="20"/>
-      <c r="DG10" s="20"/>
-      <c r="DH10" s="20"/>
+      <c r="CS10" s="76"/>
+      <c r="CT10" s="68"/>
+      <c r="CU10" s="68"/>
+      <c r="CV10" s="68"/>
+      <c r="CW10" s="68"/>
+      <c r="CX10" s="68"/>
+      <c r="CY10" s="68"/>
+      <c r="CZ10" s="68"/>
+      <c r="DA10" s="68"/>
+      <c r="DB10" s="68"/>
+      <c r="DC10" s="68"/>
+      <c r="DD10" s="68"/>
+      <c r="DE10" s="68"/>
+      <c r="DF10" s="68"/>
+      <c r="DG10" s="68"/>
+      <c r="DH10" s="68"/>
     </row>
     <row r="11" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="22">
         <v>44098</v>
@@ -2512,7 +2662,7 @@
       <c r="G11" s="24">
         <v>1</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
@@ -2601,160 +2751,164 @@
       <c r="CP11" s="30"/>
       <c r="CQ11" s="30"/>
       <c r="CR11" s="30"/>
-      <c r="CS11" s="30"/>
-      <c r="CT11" s="30"/>
-      <c r="CU11" s="30"/>
-      <c r="CV11" s="30"/>
-      <c r="CW11" s="30"/>
-      <c r="CX11" s="30"/>
-      <c r="CY11" s="32"/>
-      <c r="CZ11" s="32"/>
-      <c r="DA11" s="32"/>
-      <c r="DB11" s="32"/>
-      <c r="DC11" s="32"/>
-      <c r="DD11" s="30"/>
-      <c r="DE11" s="30"/>
-      <c r="DF11" s="30"/>
-      <c r="DG11" s="30"/>
-      <c r="DH11" s="30"/>
+      <c r="CS11" s="79"/>
+      <c r="CT11" s="68"/>
+      <c r="CU11" s="68"/>
+      <c r="CV11" s="68"/>
+      <c r="CW11" s="68"/>
+      <c r="CX11" s="68"/>
+      <c r="CY11" s="68"/>
+      <c r="CZ11" s="68"/>
+      <c r="DA11" s="68"/>
+      <c r="DB11" s="68"/>
+      <c r="DC11" s="68"/>
+      <c r="DD11" s="68"/>
+      <c r="DE11" s="68"/>
+      <c r="DF11" s="68"/>
+      <c r="DG11" s="68"/>
+      <c r="DH11" s="68"/>
     </row>
     <row r="12" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="D12" s="22">
+        <v>44098</v>
+      </c>
+      <c r="E12" s="22">
+        <v>44186</v>
+      </c>
       <c r="F12" s="23">
         <v>87</v>
       </c>
-      <c r="G12" s="66">
-        <v>0.05</v>
-      </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="28"/>
-      <c r="AC12" s="28"/>
-      <c r="AD12" s="28"/>
-      <c r="AE12" s="28"/>
-      <c r="AF12" s="28"/>
-      <c r="AG12" s="26"/>
-      <c r="AH12" s="26"/>
-      <c r="AI12" s="26"/>
-      <c r="AJ12" s="26"/>
-      <c r="AK12" s="26"/>
-      <c r="AL12" s="26"/>
-      <c r="AM12" s="26"/>
-      <c r="AN12" s="26"/>
-      <c r="AO12" s="26"/>
-      <c r="AP12" s="26"/>
-      <c r="AQ12" s="29"/>
-      <c r="AR12" s="29"/>
-      <c r="AS12" s="29"/>
-      <c r="AT12" s="29"/>
-      <c r="AU12" s="29"/>
-      <c r="AV12" s="30"/>
-      <c r="AW12" s="30"/>
-      <c r="AX12" s="30"/>
-      <c r="AY12" s="30"/>
-      <c r="AZ12" s="30"/>
-      <c r="BA12" s="30"/>
-      <c r="BB12" s="30"/>
-      <c r="BC12" s="30"/>
-      <c r="BD12" s="30"/>
-      <c r="BE12" s="30"/>
-      <c r="BF12" s="31"/>
-      <c r="BG12" s="31"/>
-      <c r="BH12" s="31"/>
-      <c r="BI12" s="31"/>
-      <c r="BJ12" s="31"/>
-      <c r="BK12" s="30"/>
-      <c r="BL12" s="30"/>
-      <c r="BM12" s="30"/>
-      <c r="BN12" s="30"/>
-      <c r="BO12" s="30"/>
-      <c r="BP12" s="30"/>
-      <c r="BQ12" s="30"/>
-      <c r="BR12" s="30"/>
-      <c r="BS12" s="30"/>
-      <c r="BT12" s="30"/>
-      <c r="BU12" s="32"/>
-      <c r="BV12" s="32"/>
-      <c r="BW12" s="32"/>
-      <c r="BX12" s="32"/>
-      <c r="BY12" s="32"/>
-      <c r="BZ12" s="30"/>
-      <c r="CA12" s="30"/>
-      <c r="CB12" s="30"/>
-      <c r="CC12" s="30"/>
-      <c r="CD12" s="30"/>
-      <c r="CE12" s="30"/>
-      <c r="CF12" s="30"/>
-      <c r="CG12" s="30"/>
-      <c r="CH12" s="30"/>
-      <c r="CI12" s="30"/>
-      <c r="CJ12" s="32"/>
-      <c r="CK12" s="32"/>
-      <c r="CL12" s="32"/>
-      <c r="CM12" s="32"/>
-      <c r="CN12" s="32"/>
-      <c r="CO12" s="30"/>
-      <c r="CP12" s="30"/>
-      <c r="CQ12" s="30"/>
+      <c r="G12" s="44">
+        <v>1</v>
+      </c>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="67"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="67"/>
+      <c r="Z12" s="67"/>
+      <c r="AA12" s="67"/>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="67"/>
+      <c r="AD12" s="67"/>
+      <c r="AE12" s="67"/>
+      <c r="AF12" s="67"/>
+      <c r="AG12" s="67"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="67"/>
+      <c r="AJ12" s="67"/>
+      <c r="AK12" s="67"/>
+      <c r="AL12" s="67"/>
+      <c r="AM12" s="67"/>
+      <c r="AN12" s="67"/>
+      <c r="AO12" s="67"/>
+      <c r="AP12" s="67"/>
+      <c r="AQ12" s="67"/>
+      <c r="AR12" s="67"/>
+      <c r="AS12" s="67"/>
+      <c r="AT12" s="67"/>
+      <c r="AU12" s="67"/>
+      <c r="AV12" s="67"/>
+      <c r="AW12" s="67"/>
+      <c r="AX12" s="67"/>
+      <c r="AY12" s="67"/>
+      <c r="AZ12" s="67"/>
+      <c r="BA12" s="67"/>
+      <c r="BB12" s="67"/>
+      <c r="BC12" s="67"/>
+      <c r="BD12" s="67"/>
+      <c r="BE12" s="67"/>
+      <c r="BF12" s="67"/>
+      <c r="BG12" s="67"/>
+      <c r="BH12" s="67"/>
+      <c r="BI12" s="67"/>
+      <c r="BJ12" s="67"/>
+      <c r="BK12" s="67"/>
+      <c r="BL12" s="67"/>
+      <c r="BM12" s="67"/>
+      <c r="BN12" s="67"/>
+      <c r="BO12" s="67"/>
+      <c r="BP12" s="67"/>
+      <c r="BQ12" s="67"/>
+      <c r="BR12" s="67"/>
+      <c r="BS12" s="67"/>
+      <c r="BT12" s="67"/>
+      <c r="BU12" s="67"/>
+      <c r="BV12" s="67"/>
+      <c r="BW12" s="67"/>
+      <c r="BX12" s="67"/>
+      <c r="BY12" s="67"/>
+      <c r="BZ12" s="67"/>
+      <c r="CA12" s="67"/>
+      <c r="CB12" s="67"/>
+      <c r="CC12" s="67"/>
+      <c r="CD12" s="67"/>
+      <c r="CE12" s="67"/>
+      <c r="CF12" s="67"/>
+      <c r="CG12" s="67"/>
+      <c r="CH12" s="67"/>
+      <c r="CI12" s="67"/>
+      <c r="CJ12" s="67"/>
+      <c r="CK12" s="67"/>
+      <c r="CL12" s="67"/>
+      <c r="CM12" s="67"/>
+      <c r="CN12" s="67"/>
+      <c r="CO12" s="67"/>
+      <c r="CP12" s="67"/>
+      <c r="CQ12" s="84"/>
       <c r="CR12" s="30"/>
-      <c r="CS12" s="30"/>
-      <c r="CT12" s="30"/>
-      <c r="CU12" s="30"/>
-      <c r="CV12" s="30"/>
-      <c r="CW12" s="30"/>
-      <c r="CX12" s="30"/>
-      <c r="CY12" s="32"/>
-      <c r="CZ12" s="32"/>
-      <c r="DA12" s="32"/>
-      <c r="DB12" s="32"/>
-      <c r="DC12" s="32"/>
-      <c r="DD12" s="30"/>
-      <c r="DE12" s="30"/>
-      <c r="DF12" s="30"/>
-      <c r="DG12" s="30"/>
-      <c r="DH12" s="30"/>
+      <c r="CS12" s="79"/>
+      <c r="CT12" s="68"/>
+      <c r="CU12" s="68"/>
+      <c r="CV12" s="68"/>
+      <c r="CW12" s="68"/>
+      <c r="CX12" s="68"/>
+      <c r="CY12" s="68"/>
+      <c r="CZ12" s="68"/>
+      <c r="DA12" s="68"/>
+      <c r="DB12" s="68"/>
+      <c r="DC12" s="68"/>
+      <c r="DD12" s="68"/>
+      <c r="DE12" s="68"/>
+      <c r="DF12" s="68"/>
+      <c r="DG12" s="68"/>
+      <c r="DH12" s="68"/>
     </row>
     <row r="13" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="23">
         <v>0</v>
       </c>
-      <c r="G13" s="66">
-        <v>0</v>
+      <c r="G13" s="44">
+        <v>1</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
@@ -2845,41 +2999,45 @@
       <c r="CP13" s="26"/>
       <c r="CQ13" s="26"/>
       <c r="CR13" s="26"/>
-      <c r="CS13" s="26"/>
-      <c r="CT13" s="26"/>
-      <c r="CU13" s="26"/>
-      <c r="CV13" s="26"/>
-      <c r="CW13" s="26"/>
-      <c r="CX13" s="26"/>
-      <c r="CY13" s="32"/>
-      <c r="CZ13" s="32"/>
-      <c r="DA13" s="32"/>
-      <c r="DB13" s="32"/>
-      <c r="DC13" s="32"/>
-      <c r="DD13" s="30"/>
-      <c r="DE13" s="30"/>
-      <c r="DF13" s="30"/>
-      <c r="DG13" s="30"/>
-      <c r="DH13" s="30"/>
+      <c r="CS13" s="79"/>
+      <c r="CT13" s="68"/>
+      <c r="CU13" s="68"/>
+      <c r="CV13" s="68"/>
+      <c r="CW13" s="68"/>
+      <c r="CX13" s="68"/>
+      <c r="CY13" s="68"/>
+      <c r="CZ13" s="68"/>
+      <c r="DA13" s="68"/>
+      <c r="DB13" s="68"/>
+      <c r="DC13" s="68"/>
+      <c r="DD13" s="68"/>
+      <c r="DE13" s="68"/>
+      <c r="DF13" s="68"/>
+      <c r="DG13" s="68"/>
+      <c r="DH13" s="68"/>
     </row>
     <row r="14" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="D14" s="22">
+        <v>44099</v>
+      </c>
+      <c r="E14" s="22">
+        <v>44099</v>
+      </c>
       <c r="F14" s="23">
         <v>1</v>
       </c>
       <c r="G14" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="I14" s="80"/>
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
@@ -2967,22 +3125,22 @@
       <c r="CP14" s="30"/>
       <c r="CQ14" s="30"/>
       <c r="CR14" s="30"/>
-      <c r="CS14" s="30"/>
-      <c r="CT14" s="30"/>
-      <c r="CU14" s="30"/>
-      <c r="CV14" s="30"/>
-      <c r="CW14" s="30"/>
-      <c r="CX14" s="30"/>
-      <c r="CY14" s="32"/>
-      <c r="CZ14" s="32"/>
-      <c r="DA14" s="32"/>
-      <c r="DB14" s="32"/>
-      <c r="DC14" s="32"/>
-      <c r="DD14" s="30"/>
-      <c r="DE14" s="30"/>
-      <c r="DF14" s="30"/>
-      <c r="DG14" s="30"/>
-      <c r="DH14" s="30"/>
+      <c r="CS14" s="79"/>
+      <c r="CT14" s="68"/>
+      <c r="CU14" s="68"/>
+      <c r="CV14" s="68"/>
+      <c r="CW14" s="68"/>
+      <c r="CX14" s="68"/>
+      <c r="CY14" s="68"/>
+      <c r="CZ14" s="68"/>
+      <c r="DA14" s="68"/>
+      <c r="DB14" s="68"/>
+      <c r="DC14" s="68"/>
+      <c r="DD14" s="68"/>
+      <c r="DE14" s="68"/>
+      <c r="DF14" s="68"/>
+      <c r="DG14" s="68"/>
+      <c r="DH14" s="68"/>
     </row>
     <row r="15" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2990,7 +3148,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -3085,45 +3243,49 @@
       <c r="CP15" s="20"/>
       <c r="CQ15" s="20"/>
       <c r="CR15" s="20"/>
-      <c r="CS15" s="20"/>
-      <c r="CT15" s="20"/>
-      <c r="CU15" s="20"/>
-      <c r="CV15" s="20"/>
-      <c r="CW15" s="20"/>
-      <c r="CX15" s="20"/>
-      <c r="CY15" s="20"/>
-      <c r="CZ15" s="20"/>
-      <c r="DA15" s="20"/>
-      <c r="DB15" s="20"/>
-      <c r="DC15" s="20"/>
-      <c r="DD15" s="20"/>
-      <c r="DE15" s="20"/>
-      <c r="DF15" s="20"/>
-      <c r="DG15" s="20"/>
-      <c r="DH15" s="20"/>
+      <c r="CS15" s="79"/>
+      <c r="CT15" s="68"/>
+      <c r="CU15" s="68"/>
+      <c r="CV15" s="68"/>
+      <c r="CW15" s="68"/>
+      <c r="CX15" s="68"/>
+      <c r="CY15" s="68"/>
+      <c r="CZ15" s="68"/>
+      <c r="DA15" s="68"/>
+      <c r="DB15" s="68"/>
+      <c r="DC15" s="68"/>
+      <c r="DD15" s="68"/>
+      <c r="DE15" s="68"/>
+      <c r="DF15" s="68"/>
+      <c r="DG15" s="68"/>
+      <c r="DH15" s="68"/>
     </row>
     <row r="16" spans="1:112" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="D16" s="22">
+        <v>44100</v>
+      </c>
+      <c r="E16" s="22">
+        <v>44104</v>
+      </c>
       <c r="F16" s="23">
         <v>4</v>
       </c>
-      <c r="G16" s="66">
-        <v>0</v>
+      <c r="G16" s="44">
+        <v>1</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="25"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="27"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
       <c r="N16" s="27"/>
       <c r="O16" s="27"/>
       <c r="P16" s="27"/>
@@ -3207,38 +3369,42 @@
       <c r="CP16" s="30"/>
       <c r="CQ16" s="30"/>
       <c r="CR16" s="30"/>
-      <c r="CS16" s="30"/>
-      <c r="CT16" s="30"/>
-      <c r="CU16" s="30"/>
-      <c r="CV16" s="30"/>
-      <c r="CW16" s="30"/>
-      <c r="CX16" s="30"/>
-      <c r="CY16" s="32"/>
-      <c r="CZ16" s="32"/>
-      <c r="DA16" s="32"/>
-      <c r="DB16" s="32"/>
-      <c r="DC16" s="32"/>
-      <c r="DD16" s="30"/>
-      <c r="DE16" s="30"/>
-      <c r="DF16" s="30"/>
-      <c r="DG16" s="30"/>
-      <c r="DH16" s="30"/>
+      <c r="CS16" s="79"/>
+      <c r="CT16" s="68"/>
+      <c r="CU16" s="68"/>
+      <c r="CV16" s="68"/>
+      <c r="CW16" s="68"/>
+      <c r="CX16" s="68"/>
+      <c r="CY16" s="68"/>
+      <c r="CZ16" s="68"/>
+      <c r="DA16" s="68"/>
+      <c r="DB16" s="68"/>
+      <c r="DC16" s="68"/>
+      <c r="DD16" s="68"/>
+      <c r="DE16" s="68"/>
+      <c r="DF16" s="68"/>
+      <c r="DG16" s="68"/>
+      <c r="DH16" s="68"/>
     </row>
     <row r="17" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
+        <v>47</v>
+      </c>
+      <c r="D17" s="22">
+        <v>44105</v>
+      </c>
+      <c r="E17" s="22">
+        <v>44112</v>
+      </c>
       <c r="F17" s="23">
         <v>8</v>
       </c>
-      <c r="G17" s="66">
-        <v>0</v>
+      <c r="G17" s="44">
+        <v>1</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="25"/>
@@ -3246,14 +3412,14 @@
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
       <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="82"/>
       <c r="V17" s="26"/>
       <c r="W17" s="26"/>
       <c r="X17" s="26"/>
@@ -3329,38 +3495,42 @@
       <c r="CP17" s="30"/>
       <c r="CQ17" s="30"/>
       <c r="CR17" s="30"/>
-      <c r="CS17" s="30"/>
-      <c r="CT17" s="30"/>
-      <c r="CU17" s="30"/>
-      <c r="CV17" s="30"/>
-      <c r="CW17" s="30"/>
-      <c r="CX17" s="30"/>
-      <c r="CY17" s="32"/>
-      <c r="CZ17" s="32"/>
-      <c r="DA17" s="32"/>
-      <c r="DB17" s="32"/>
-      <c r="DC17" s="32"/>
-      <c r="DD17" s="30"/>
-      <c r="DE17" s="30"/>
-      <c r="DF17" s="30"/>
-      <c r="DG17" s="30"/>
-      <c r="DH17" s="30"/>
+      <c r="CS17" s="79"/>
+      <c r="CT17" s="68"/>
+      <c r="CU17" s="68"/>
+      <c r="CV17" s="68"/>
+      <c r="CW17" s="68"/>
+      <c r="CX17" s="68"/>
+      <c r="CY17" s="68"/>
+      <c r="CZ17" s="68"/>
+      <c r="DA17" s="68"/>
+      <c r="DB17" s="68"/>
+      <c r="DC17" s="68"/>
+      <c r="DD17" s="68"/>
+      <c r="DE17" s="68"/>
+      <c r="DF17" s="68"/>
+      <c r="DG17" s="68"/>
+      <c r="DH17" s="68"/>
     </row>
     <row r="18" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
+        <v>72</v>
+      </c>
+      <c r="D18" s="22">
+        <v>44113</v>
+      </c>
+      <c r="E18" s="22">
+        <v>44124</v>
+      </c>
       <c r="F18" s="23">
         <v>12</v>
       </c>
-      <c r="G18" s="66">
-        <v>0</v>
+      <c r="G18" s="44">
+        <v>1</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="25"/>
@@ -3376,18 +3546,18 @@
       <c r="S18" s="26"/>
       <c r="T18" s="26"/>
       <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28"/>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
-      <c r="AG18" s="26"/>
+      <c r="V18" s="81"/>
+      <c r="W18" s="81"/>
+      <c r="X18" s="81"/>
+      <c r="Y18" s="81"/>
+      <c r="Z18" s="81"/>
+      <c r="AA18" s="81"/>
+      <c r="AB18" s="81"/>
+      <c r="AC18" s="81"/>
+      <c r="AD18" s="81"/>
+      <c r="AE18" s="81"/>
+      <c r="AF18" s="81"/>
+      <c r="AG18" s="81"/>
       <c r="AH18" s="26"/>
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
@@ -3451,38 +3621,42 @@
       <c r="CP18" s="30"/>
       <c r="CQ18" s="30"/>
       <c r="CR18" s="30"/>
-      <c r="CS18" s="30"/>
-      <c r="CT18" s="30"/>
-      <c r="CU18" s="30"/>
-      <c r="CV18" s="30"/>
-      <c r="CW18" s="30"/>
-      <c r="CX18" s="30"/>
-      <c r="CY18" s="32"/>
-      <c r="CZ18" s="32"/>
-      <c r="DA18" s="32"/>
-      <c r="DB18" s="32"/>
-      <c r="DC18" s="32"/>
-      <c r="DD18" s="30"/>
-      <c r="DE18" s="30"/>
-      <c r="DF18" s="30"/>
-      <c r="DG18" s="30"/>
-      <c r="DH18" s="30"/>
+      <c r="CS18" s="79"/>
+      <c r="CT18" s="68"/>
+      <c r="CU18" s="68"/>
+      <c r="CV18" s="68"/>
+      <c r="CW18" s="68"/>
+      <c r="CX18" s="68"/>
+      <c r="CY18" s="68"/>
+      <c r="CZ18" s="68"/>
+      <c r="DA18" s="68"/>
+      <c r="DB18" s="68"/>
+      <c r="DC18" s="68"/>
+      <c r="DD18" s="68"/>
+      <c r="DE18" s="68"/>
+      <c r="DF18" s="68"/>
+      <c r="DG18" s="68"/>
+      <c r="DH18" s="68"/>
     </row>
     <row r="19" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
+        <v>71</v>
+      </c>
+      <c r="D19" s="22">
+        <v>44125</v>
+      </c>
+      <c r="E19" s="22">
+        <v>44136</v>
+      </c>
       <c r="F19" s="23">
         <v>12</v>
       </c>
-      <c r="G19" s="66">
-        <v>0</v>
+      <c r="G19" s="44">
+        <v>1</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="25"/>
@@ -3510,18 +3684,18 @@
       <c r="AE19" s="28"/>
       <c r="AF19" s="28"/>
       <c r="AG19" s="26"/>
-      <c r="AH19" s="26"/>
-      <c r="AI19" s="26"/>
-      <c r="AJ19" s="26"/>
-      <c r="AK19" s="26"/>
-      <c r="AL19" s="26"/>
-      <c r="AM19" s="26"/>
-      <c r="AN19" s="26"/>
-      <c r="AO19" s="26"/>
-      <c r="AP19" s="26"/>
-      <c r="AQ19" s="29"/>
-      <c r="AR19" s="29"/>
-      <c r="AS19" s="29"/>
+      <c r="AH19" s="81"/>
+      <c r="AI19" s="81"/>
+      <c r="AJ19" s="81"/>
+      <c r="AK19" s="81"/>
+      <c r="AL19" s="81"/>
+      <c r="AM19" s="81"/>
+      <c r="AN19" s="81"/>
+      <c r="AO19" s="81"/>
+      <c r="AP19" s="81"/>
+      <c r="AQ19" s="81"/>
+      <c r="AR19" s="81"/>
+      <c r="AS19" s="81"/>
       <c r="AT19" s="29"/>
       <c r="AU19" s="29"/>
       <c r="AV19" s="30"/>
@@ -3573,22 +3747,22 @@
       <c r="CP19" s="30"/>
       <c r="CQ19" s="30"/>
       <c r="CR19" s="30"/>
-      <c r="CS19" s="30"/>
-      <c r="CT19" s="30"/>
-      <c r="CU19" s="30"/>
-      <c r="CV19" s="30"/>
-      <c r="CW19" s="30"/>
-      <c r="CX19" s="30"/>
-      <c r="CY19" s="32"/>
-      <c r="CZ19" s="32"/>
-      <c r="DA19" s="32"/>
-      <c r="DB19" s="32"/>
-      <c r="DC19" s="32"/>
-      <c r="DD19" s="30"/>
-      <c r="DE19" s="30"/>
-      <c r="DF19" s="30"/>
-      <c r="DG19" s="30"/>
-      <c r="DH19" s="30"/>
+      <c r="CS19" s="79"/>
+      <c r="CT19" s="68"/>
+      <c r="CU19" s="68"/>
+      <c r="CV19" s="68"/>
+      <c r="CW19" s="68"/>
+      <c r="CX19" s="68"/>
+      <c r="CY19" s="68"/>
+      <c r="CZ19" s="68"/>
+      <c r="DA19" s="68"/>
+      <c r="DB19" s="68"/>
+      <c r="DC19" s="68"/>
+      <c r="DD19" s="68"/>
+      <c r="DE19" s="68"/>
+      <c r="DF19" s="68"/>
+      <c r="DG19" s="68"/>
+      <c r="DH19" s="68"/>
     </row>
     <row r="20" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -3596,7 +3770,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -3691,38 +3865,42 @@
       <c r="CP20" s="20"/>
       <c r="CQ20" s="20"/>
       <c r="CR20" s="20"/>
-      <c r="CS20" s="20"/>
-      <c r="CT20" s="20"/>
-      <c r="CU20" s="20"/>
-      <c r="CV20" s="20"/>
-      <c r="CW20" s="20"/>
-      <c r="CX20" s="20"/>
-      <c r="CY20" s="20"/>
-      <c r="CZ20" s="20"/>
-      <c r="DA20" s="20"/>
-      <c r="DB20" s="20"/>
-      <c r="DC20" s="20"/>
-      <c r="DD20" s="20"/>
-      <c r="DE20" s="20"/>
-      <c r="DF20" s="20"/>
-      <c r="DG20" s="20"/>
-      <c r="DH20" s="20"/>
+      <c r="CS20" s="79"/>
+      <c r="CT20" s="68"/>
+      <c r="CU20" s="68"/>
+      <c r="CV20" s="68"/>
+      <c r="CW20" s="68"/>
+      <c r="CX20" s="68"/>
+      <c r="CY20" s="68"/>
+      <c r="CZ20" s="68"/>
+      <c r="DA20" s="68"/>
+      <c r="DB20" s="68"/>
+      <c r="DC20" s="68"/>
+      <c r="DD20" s="68"/>
+      <c r="DE20" s="68"/>
+      <c r="DF20" s="68"/>
+      <c r="DG20" s="68"/>
+      <c r="DH20" s="68"/>
     </row>
     <row r="21" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+        <v>46</v>
+      </c>
+      <c r="D21" s="22">
+        <v>44137</v>
+      </c>
+      <c r="E21" s="22">
+        <v>44140</v>
+      </c>
       <c r="F21" s="23">
         <v>4</v>
       </c>
       <c r="G21" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="34"/>
       <c r="I21" s="25"/>
@@ -3762,10 +3940,10 @@
       <c r="AQ21" s="29"/>
       <c r="AR21" s="29"/>
       <c r="AS21" s="29"/>
-      <c r="AT21" s="29"/>
-      <c r="AU21" s="29"/>
-      <c r="AV21" s="30"/>
-      <c r="AW21" s="30"/>
+      <c r="AT21" s="83"/>
+      <c r="AU21" s="83"/>
+      <c r="AV21" s="83"/>
+      <c r="AW21" s="83"/>
       <c r="AX21" s="30"/>
       <c r="AY21" s="30"/>
       <c r="AZ21" s="30"/>
@@ -3813,38 +3991,42 @@
       <c r="CP21" s="30"/>
       <c r="CQ21" s="30"/>
       <c r="CR21" s="30"/>
-      <c r="CS21" s="30"/>
-      <c r="CT21" s="30"/>
-      <c r="CU21" s="30"/>
-      <c r="CV21" s="30"/>
-      <c r="CW21" s="30"/>
-      <c r="CX21" s="30"/>
-      <c r="CY21" s="32"/>
-      <c r="CZ21" s="32"/>
-      <c r="DA21" s="32"/>
-      <c r="DB21" s="32"/>
-      <c r="DC21" s="32"/>
-      <c r="DD21" s="30"/>
-      <c r="DE21" s="30"/>
-      <c r="DF21" s="30"/>
-      <c r="DG21" s="30"/>
-      <c r="DH21" s="30"/>
+      <c r="CS21" s="79"/>
+      <c r="CT21" s="68"/>
+      <c r="CU21" s="68"/>
+      <c r="CV21" s="68"/>
+      <c r="CW21" s="68"/>
+      <c r="CX21" s="68"/>
+      <c r="CY21" s="68"/>
+      <c r="CZ21" s="68"/>
+      <c r="DA21" s="68"/>
+      <c r="DB21" s="68"/>
+      <c r="DC21" s="68"/>
+      <c r="DD21" s="68"/>
+      <c r="DE21" s="68"/>
+      <c r="DF21" s="68"/>
+      <c r="DG21" s="68"/>
+      <c r="DH21" s="68"/>
     </row>
     <row r="22" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
+        <v>49</v>
+      </c>
+      <c r="D22" s="22">
+        <v>44141</v>
+      </c>
+      <c r="E22" s="22">
+        <v>44148</v>
+      </c>
       <c r="F22" s="23">
         <v>8</v>
       </c>
       <c r="G22" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="34"/>
       <c r="I22" s="25"/>
@@ -3888,14 +4070,14 @@
       <c r="AU22" s="29"/>
       <c r="AV22" s="30"/>
       <c r="AW22" s="30"/>
-      <c r="AX22" s="30"/>
-      <c r="AY22" s="30"/>
-      <c r="AZ22" s="30"/>
-      <c r="BA22" s="30"/>
-      <c r="BB22" s="30"/>
-      <c r="BC22" s="30"/>
-      <c r="BD22" s="30"/>
-      <c r="BE22" s="30"/>
+      <c r="AX22" s="84"/>
+      <c r="AY22" s="84"/>
+      <c r="AZ22" s="84"/>
+      <c r="BA22" s="84"/>
+      <c r="BB22" s="84"/>
+      <c r="BC22" s="84"/>
+      <c r="BD22" s="84"/>
+      <c r="BE22" s="84"/>
       <c r="BF22" s="31"/>
       <c r="BG22" s="31"/>
       <c r="BH22" s="31"/>
@@ -3935,38 +4117,42 @@
       <c r="CP22" s="30"/>
       <c r="CQ22" s="30"/>
       <c r="CR22" s="30"/>
-      <c r="CS22" s="30"/>
-      <c r="CT22" s="30"/>
-      <c r="CU22" s="30"/>
-      <c r="CV22" s="30"/>
-      <c r="CW22" s="30"/>
-      <c r="CX22" s="30"/>
-      <c r="CY22" s="32"/>
-      <c r="CZ22" s="32"/>
-      <c r="DA22" s="32"/>
-      <c r="DB22" s="32"/>
-      <c r="DC22" s="32"/>
-      <c r="DD22" s="30"/>
-      <c r="DE22" s="30"/>
-      <c r="DF22" s="30"/>
-      <c r="DG22" s="30"/>
-      <c r="DH22" s="30"/>
+      <c r="CS22" s="79"/>
+      <c r="CT22" s="68"/>
+      <c r="CU22" s="68"/>
+      <c r="CV22" s="68"/>
+      <c r="CW22" s="68"/>
+      <c r="CX22" s="68"/>
+      <c r="CY22" s="68"/>
+      <c r="CZ22" s="68"/>
+      <c r="DA22" s="68"/>
+      <c r="DB22" s="68"/>
+      <c r="DC22" s="68"/>
+      <c r="DD22" s="68"/>
+      <c r="DE22" s="68"/>
+      <c r="DF22" s="68"/>
+      <c r="DG22" s="68"/>
+      <c r="DH22" s="68"/>
     </row>
     <row r="23" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
+        <v>69</v>
+      </c>
+      <c r="D23" s="22">
+        <v>44149</v>
+      </c>
+      <c r="E23" s="22">
+        <v>44164</v>
+      </c>
       <c r="F23" s="23">
         <v>15</v>
       </c>
       <c r="G23" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="34"/>
       <c r="I23" s="25"/>
@@ -4018,21 +4204,21 @@
       <c r="BC23" s="30"/>
       <c r="BD23" s="30"/>
       <c r="BE23" s="30"/>
-      <c r="BF23" s="31"/>
-      <c r="BG23" s="31"/>
-      <c r="BH23" s="31"/>
-      <c r="BI23" s="31"/>
-      <c r="BJ23" s="31"/>
-      <c r="BK23" s="30"/>
-      <c r="BL23" s="30"/>
-      <c r="BM23" s="30"/>
-      <c r="BN23" s="30"/>
-      <c r="BO23" s="30"/>
-      <c r="BP23" s="30"/>
-      <c r="BQ23" s="63"/>
-      <c r="BR23" s="63"/>
-      <c r="BS23" s="63"/>
-      <c r="BT23" s="63"/>
+      <c r="BF23" s="85"/>
+      <c r="BG23" s="85"/>
+      <c r="BH23" s="85"/>
+      <c r="BI23" s="85"/>
+      <c r="BJ23" s="85"/>
+      <c r="BK23" s="85"/>
+      <c r="BL23" s="85"/>
+      <c r="BM23" s="85"/>
+      <c r="BN23" s="85"/>
+      <c r="BO23" s="85"/>
+      <c r="BP23" s="85"/>
+      <c r="BQ23" s="85"/>
+      <c r="BR23" s="85"/>
+      <c r="BS23" s="85"/>
+      <c r="BT23" s="85"/>
       <c r="BU23" s="32"/>
       <c r="BV23" s="32"/>
       <c r="BW23" s="32"/>
@@ -4057,38 +4243,42 @@
       <c r="CP23" s="30"/>
       <c r="CQ23" s="30"/>
       <c r="CR23" s="30"/>
-      <c r="CS23" s="30"/>
-      <c r="CT23" s="30"/>
-      <c r="CU23" s="30"/>
-      <c r="CV23" s="30"/>
-      <c r="CW23" s="30"/>
-      <c r="CX23" s="30"/>
-      <c r="CY23" s="32"/>
-      <c r="CZ23" s="32"/>
-      <c r="DA23" s="32"/>
-      <c r="DB23" s="32"/>
-      <c r="DC23" s="32"/>
-      <c r="DD23" s="30"/>
-      <c r="DE23" s="30"/>
-      <c r="DF23" s="30"/>
-      <c r="DG23" s="30"/>
-      <c r="DH23" s="30"/>
+      <c r="CS23" s="79"/>
+      <c r="CT23" s="68"/>
+      <c r="CU23" s="68"/>
+      <c r="CV23" s="68"/>
+      <c r="CW23" s="68"/>
+      <c r="CX23" s="68"/>
+      <c r="CY23" s="68"/>
+      <c r="CZ23" s="68"/>
+      <c r="DA23" s="68"/>
+      <c r="DB23" s="68"/>
+      <c r="DC23" s="68"/>
+      <c r="DD23" s="68"/>
+      <c r="DE23" s="68"/>
+      <c r="DF23" s="68"/>
+      <c r="DG23" s="68"/>
+      <c r="DH23" s="68"/>
     </row>
     <row r="24" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
+        <v>70</v>
+      </c>
+      <c r="D24" s="22">
+        <v>44165</v>
+      </c>
+      <c r="E24" s="22">
+        <v>44179</v>
+      </c>
       <c r="F24" s="23">
         <v>15</v>
       </c>
       <c r="G24" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="34"/>
       <c r="I24" s="25"/>
@@ -4155,46 +4345,46 @@
       <c r="BR24" s="30"/>
       <c r="BS24" s="30"/>
       <c r="BT24" s="30"/>
-      <c r="BU24" s="32"/>
-      <c r="BV24" s="32"/>
-      <c r="BW24" s="32"/>
-      <c r="BX24" s="32"/>
-      <c r="BY24" s="32"/>
-      <c r="BZ24" s="30"/>
-      <c r="CA24" s="30"/>
-      <c r="CB24" s="30"/>
-      <c r="CC24" s="30"/>
-      <c r="CD24" s="30"/>
-      <c r="CE24" s="63"/>
-      <c r="CF24" s="63"/>
-      <c r="CG24" s="63"/>
-      <c r="CH24" s="63"/>
-      <c r="CI24" s="63"/>
+      <c r="BU24" s="86"/>
+      <c r="BV24" s="86"/>
+      <c r="BW24" s="86"/>
+      <c r="BX24" s="86"/>
+      <c r="BY24" s="86"/>
+      <c r="BZ24" s="86"/>
+      <c r="CA24" s="86"/>
+      <c r="CB24" s="86"/>
+      <c r="CC24" s="86"/>
+      <c r="CD24" s="86"/>
+      <c r="CE24" s="86"/>
+      <c r="CF24" s="86"/>
+      <c r="CG24" s="86"/>
+      <c r="CH24" s="86"/>
+      <c r="CI24" s="86"/>
       <c r="CJ24" s="32"/>
       <c r="CK24" s="32"/>
       <c r="CL24" s="32"/>
       <c r="CM24" s="32"/>
       <c r="CN24" s="32"/>
-      <c r="CO24" s="63"/>
-      <c r="CP24" s="63"/>
-      <c r="CQ24" s="63"/>
-      <c r="CR24" s="63"/>
-      <c r="CS24" s="63"/>
-      <c r="CT24" s="63"/>
-      <c r="CU24" s="30"/>
-      <c r="CV24" s="30"/>
-      <c r="CW24" s="30"/>
-      <c r="CX24" s="30"/>
-      <c r="CY24" s="32"/>
-      <c r="CZ24" s="32"/>
-      <c r="DA24" s="32"/>
-      <c r="DB24" s="32"/>
-      <c r="DC24" s="32"/>
-      <c r="DD24" s="30"/>
-      <c r="DE24" s="30"/>
-      <c r="DF24" s="30"/>
-      <c r="DG24" s="30"/>
-      <c r="DH24" s="30"/>
+      <c r="CO24" s="41"/>
+      <c r="CP24" s="41"/>
+      <c r="CQ24" s="41"/>
+      <c r="CR24" s="41"/>
+      <c r="CS24" s="79"/>
+      <c r="CT24" s="68"/>
+      <c r="CU24" s="68"/>
+      <c r="CV24" s="68"/>
+      <c r="CW24" s="68"/>
+      <c r="CX24" s="68"/>
+      <c r="CY24" s="68"/>
+      <c r="CZ24" s="68"/>
+      <c r="DA24" s="68"/>
+      <c r="DB24" s="68"/>
+      <c r="DC24" s="68"/>
+      <c r="DD24" s="68"/>
+      <c r="DE24" s="68"/>
+      <c r="DF24" s="68"/>
+      <c r="DG24" s="68"/>
+      <c r="DH24" s="68"/>
     </row>
     <row r="25" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -4202,7 +4392,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -4288,47 +4478,51 @@
       <c r="CG25" s="20"/>
       <c r="CH25" s="20"/>
       <c r="CI25" s="20"/>
-      <c r="CJ25" s="20"/>
-      <c r="CK25" s="20"/>
-      <c r="CL25" s="20"/>
-      <c r="CM25" s="20"/>
+      <c r="CJ25" s="87"/>
+      <c r="CK25" s="87"/>
+      <c r="CL25" s="87"/>
+      <c r="CM25" s="87"/>
       <c r="CN25" s="20"/>
       <c r="CO25" s="20"/>
       <c r="CP25" s="20"/>
       <c r="CQ25" s="20"/>
       <c r="CR25" s="20"/>
-      <c r="CS25" s="20"/>
-      <c r="CT25" s="20"/>
-      <c r="CU25" s="20"/>
-      <c r="CV25" s="20"/>
-      <c r="CW25" s="20"/>
-      <c r="CX25" s="20"/>
-      <c r="CY25" s="20"/>
-      <c r="CZ25" s="20"/>
-      <c r="DA25" s="20"/>
-      <c r="DB25" s="20"/>
-      <c r="DC25" s="20"/>
-      <c r="DD25" s="20"/>
-      <c r="DE25" s="20"/>
-      <c r="DF25" s="20"/>
-      <c r="DG25" s="20"/>
-      <c r="DH25" s="20"/>
+      <c r="CS25" s="79"/>
+      <c r="CT25" s="68"/>
+      <c r="CU25" s="68"/>
+      <c r="CV25" s="68"/>
+      <c r="CW25" s="68"/>
+      <c r="CX25" s="68"/>
+      <c r="CY25" s="68"/>
+      <c r="CZ25" s="68"/>
+      <c r="DA25" s="68"/>
+      <c r="DB25" s="68"/>
+      <c r="DC25" s="68"/>
+      <c r="DD25" s="68"/>
+      <c r="DE25" s="68"/>
+      <c r="DF25" s="68"/>
+      <c r="DG25" s="68"/>
+      <c r="DH25" s="68"/>
     </row>
     <row r="26" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+        <v>53</v>
+      </c>
+      <c r="D26" s="22">
+        <v>44180</v>
+      </c>
+      <c r="E26" s="22">
+        <v>44183</v>
+      </c>
       <c r="F26" s="23">
         <v>4</v>
       </c>
       <c r="G26" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="34"/>
       <c r="I26" s="25"/>
@@ -4414,43 +4608,47 @@
       <c r="CK26" s="32"/>
       <c r="CL26" s="32"/>
       <c r="CM26" s="32"/>
-      <c r="CN26" s="32"/>
-      <c r="CO26" s="62"/>
-      <c r="CP26" s="62"/>
-      <c r="CQ26" s="62"/>
-      <c r="CR26" s="62"/>
-      <c r="CS26" s="62"/>
-      <c r="CT26" s="62"/>
-      <c r="CU26" s="62"/>
-      <c r="CV26" s="62"/>
-      <c r="CW26" s="62"/>
-      <c r="CX26" s="62"/>
-      <c r="CY26" s="32"/>
-      <c r="CZ26" s="32"/>
-      <c r="DA26" s="32"/>
-      <c r="DB26" s="32"/>
-      <c r="DC26" s="32"/>
-      <c r="DD26" s="30"/>
-      <c r="DE26" s="30"/>
-      <c r="DF26" s="30"/>
-      <c r="DG26" s="30"/>
-      <c r="DH26" s="30"/>
+      <c r="CN26" s="88"/>
+      <c r="CO26" s="88"/>
+      <c r="CP26" s="88"/>
+      <c r="CQ26" s="88"/>
+      <c r="CR26" s="40"/>
+      <c r="CS26" s="79"/>
+      <c r="CT26" s="68"/>
+      <c r="CU26" s="68"/>
+      <c r="CV26" s="68"/>
+      <c r="CW26" s="68"/>
+      <c r="CX26" s="68"/>
+      <c r="CY26" s="68"/>
+      <c r="CZ26" s="68"/>
+      <c r="DA26" s="68"/>
+      <c r="DB26" s="68"/>
+      <c r="DC26" s="68"/>
+      <c r="DD26" s="68"/>
+      <c r="DE26" s="68"/>
+      <c r="DF26" s="68"/>
+      <c r="DG26" s="68"/>
+      <c r="DH26" s="68"/>
     </row>
     <row r="27" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+        <v>54</v>
+      </c>
+      <c r="D27" s="22">
+        <v>44184</v>
+      </c>
+      <c r="E27" s="22">
+        <v>44186</v>
+      </c>
       <c r="F27" s="23">
         <v>4</v>
       </c>
       <c r="G27" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="34"/>
       <c r="I27" s="25"/>
@@ -4541,22 +4739,22 @@
       <c r="CP27" s="30"/>
       <c r="CQ27" s="30"/>
       <c r="CR27" s="30"/>
-      <c r="CS27" s="30"/>
-      <c r="CT27" s="30"/>
-      <c r="CU27" s="30"/>
-      <c r="CV27" s="30"/>
-      <c r="CW27" s="30"/>
-      <c r="CX27" s="30"/>
-      <c r="CY27" s="32"/>
-      <c r="CZ27" s="32"/>
-      <c r="DA27" s="32"/>
-      <c r="DB27" s="32"/>
-      <c r="DC27" s="32"/>
-      <c r="DD27" s="62"/>
-      <c r="DE27" s="62"/>
-      <c r="DF27" s="62"/>
-      <c r="DG27" s="62"/>
-      <c r="DH27" s="62"/>
+      <c r="CS27" s="79"/>
+      <c r="CT27" s="68"/>
+      <c r="CU27" s="68"/>
+      <c r="CV27" s="68"/>
+      <c r="CW27" s="68"/>
+      <c r="CX27" s="68"/>
+      <c r="CY27" s="68"/>
+      <c r="CZ27" s="68"/>
+      <c r="DA27" s="68"/>
+      <c r="DB27" s="68"/>
+      <c r="DC27" s="68"/>
+      <c r="DD27" s="68"/>
+      <c r="DE27" s="68"/>
+      <c r="DF27" s="68"/>
+      <c r="DG27" s="68"/>
+      <c r="DH27" s="68"/>
     </row>
     <row r="28" spans="1:133" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -4629,168 +4827,141 @@
     </row>
     <row r="29" spans="1:133" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="39"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="39"/>
-      <c r="AC29" s="39"/>
-      <c r="AD29" s="39"/>
-      <c r="AE29" s="39"/>
-      <c r="AF29" s="39"/>
-      <c r="AG29" s="39"/>
-      <c r="AH29" s="39"/>
-      <c r="AI29" s="39"/>
-      <c r="AJ29" s="39"/>
-      <c r="AK29" s="39"/>
-      <c r="AL29" s="39"/>
-      <c r="AM29" s="39"/>
-      <c r="AN29" s="39"/>
-      <c r="AO29" s="39"/>
-      <c r="AP29" s="39"/>
-      <c r="AQ29" s="39"/>
-      <c r="AR29" s="39"/>
-      <c r="AS29" s="39"/>
-      <c r="AT29" s="39"/>
-      <c r="AU29" s="39"/>
-      <c r="AV29" s="39"/>
-      <c r="AW29" s="39"/>
-      <c r="AX29" s="39"/>
-      <c r="AY29" s="39"/>
-      <c r="AZ29" s="39"/>
-      <c r="BA29" s="39"/>
-      <c r="BB29" s="39"/>
-      <c r="BC29" s="39"/>
-      <c r="BD29" s="39"/>
-      <c r="BE29" s="39"/>
-      <c r="BF29" s="39"/>
-      <c r="BG29" s="39"/>
-      <c r="BH29" s="39"/>
-      <c r="BI29" s="39"/>
-      <c r="BJ29" s="39"/>
-      <c r="BK29" s="39"/>
-      <c r="BL29" s="39"/>
-      <c r="BM29" s="39"/>
-      <c r="BN29" s="39"/>
-      <c r="BO29" s="39"/>
-      <c r="BP29" s="65"/>
-      <c r="BQ29" s="65"/>
-      <c r="BR29" s="65"/>
-      <c r="BS29" s="65"/>
-      <c r="BT29" s="65"/>
-      <c r="BU29" s="65"/>
-      <c r="BV29" s="65"/>
-      <c r="BW29" s="65"/>
-      <c r="BX29" s="65"/>
-      <c r="BY29" s="65"/>
-      <c r="BZ29" s="65"/>
-      <c r="CA29" s="65"/>
-      <c r="CB29" s="65"/>
-      <c r="CC29" s="65"/>
-      <c r="CD29" s="65"/>
-      <c r="CE29" s="65"/>
-      <c r="CF29" s="65"/>
-      <c r="CG29" s="65"/>
-      <c r="CH29" s="65"/>
-      <c r="CI29" s="65"/>
-      <c r="CJ29" s="65"/>
-      <c r="CK29" s="65"/>
-      <c r="CL29" s="65"/>
-      <c r="CM29" s="65"/>
-      <c r="CN29" s="65"/>
-      <c r="CO29" s="65"/>
-      <c r="CP29" s="65"/>
-      <c r="CQ29" s="65"/>
-      <c r="CR29" s="65"/>
-      <c r="CS29" s="65"/>
-      <c r="CT29" s="65"/>
-      <c r="CU29" s="65"/>
-      <c r="CV29" s="65"/>
-      <c r="CW29" s="65"/>
-      <c r="CX29" s="65"/>
-      <c r="CY29" s="65"/>
-      <c r="CZ29" s="65"/>
-      <c r="DA29" s="65"/>
-      <c r="DB29" s="65"/>
-      <c r="DC29" s="65"/>
-      <c r="DD29" s="65"/>
-      <c r="DE29" s="65"/>
-      <c r="DF29" s="65"/>
-      <c r="DG29" s="65"/>
-      <c r="DH29" s="65"/>
-      <c r="DI29" s="64"/>
-      <c r="DJ29" s="64"/>
-      <c r="DK29" s="64"/>
-      <c r="DL29" s="64"/>
-      <c r="DM29" s="64"/>
-      <c r="DN29" s="64"/>
-      <c r="DO29" s="64"/>
-      <c r="DP29" s="64"/>
-      <c r="DQ29" s="64"/>
-      <c r="DR29" s="64"/>
-      <c r="DS29" s="64"/>
-      <c r="DT29" s="64"/>
-      <c r="DU29" s="64"/>
-      <c r="DV29" s="64"/>
-      <c r="DW29" s="64"/>
-      <c r="DX29" s="64"/>
-      <c r="DY29" s="64"/>
-      <c r="DZ29" s="64"/>
-      <c r="EA29" s="64"/>
-      <c r="EB29" s="64"/>
-      <c r="EC29" s="64"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="64"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="64"/>
+      <c r="U29" s="64"/>
+      <c r="V29" s="64"/>
+      <c r="W29" s="64"/>
+      <c r="X29" s="64"/>
+      <c r="Y29" s="64"/>
+      <c r="Z29" s="64"/>
+      <c r="AA29" s="64"/>
+      <c r="AB29" s="64"/>
+      <c r="AC29" s="64"/>
+      <c r="AD29" s="64"/>
+      <c r="AE29" s="64"/>
+      <c r="AF29" s="64"/>
+      <c r="AG29" s="64"/>
+      <c r="AH29" s="64"/>
+      <c r="AI29" s="64"/>
+      <c r="AJ29" s="64"/>
+      <c r="AK29" s="64"/>
+      <c r="AL29" s="64"/>
+      <c r="AM29" s="64"/>
+      <c r="AN29" s="64"/>
+      <c r="AO29" s="64"/>
+      <c r="AP29" s="64"/>
+      <c r="AQ29" s="64"/>
+      <c r="AR29" s="64"/>
+      <c r="AS29" s="64"/>
+      <c r="AT29" s="64"/>
+      <c r="AU29" s="64"/>
+      <c r="AV29" s="64"/>
+      <c r="AW29" s="64"/>
+      <c r="AX29" s="64"/>
+      <c r="AY29" s="64"/>
+      <c r="AZ29" s="64"/>
+      <c r="BA29" s="64"/>
+      <c r="BB29" s="64"/>
+      <c r="BC29" s="64"/>
+      <c r="BD29" s="64"/>
+      <c r="BE29" s="64"/>
+      <c r="BF29" s="64"/>
+      <c r="BG29" s="64"/>
+      <c r="BH29" s="64"/>
+      <c r="BI29" s="64"/>
+      <c r="BJ29" s="64"/>
+      <c r="BK29" s="64"/>
+      <c r="BL29" s="64"/>
+      <c r="BM29" s="64"/>
+      <c r="BN29" s="64"/>
+      <c r="BO29" s="64"/>
+      <c r="BP29" s="43"/>
+      <c r="BQ29" s="43"/>
+      <c r="BR29" s="43"/>
+      <c r="BS29" s="43"/>
+      <c r="BT29" s="43"/>
+      <c r="BU29" s="43"/>
+      <c r="BV29" s="43"/>
+      <c r="BW29" s="43"/>
+      <c r="BX29" s="43"/>
+      <c r="BY29" s="43"/>
+      <c r="BZ29" s="43"/>
+      <c r="CA29" s="43"/>
+      <c r="CB29" s="43"/>
+      <c r="CC29" s="43"/>
+      <c r="CD29" s="43"/>
+      <c r="CE29" s="43"/>
+      <c r="CF29" s="43"/>
+      <c r="CG29" s="43"/>
+      <c r="CH29" s="43"/>
+      <c r="CI29" s="43"/>
+      <c r="CJ29" s="43"/>
+      <c r="CK29" s="43"/>
+      <c r="CL29" s="43"/>
+      <c r="CM29" s="43"/>
+      <c r="CN29" s="43"/>
+      <c r="CO29" s="43"/>
+      <c r="CP29" s="43"/>
+      <c r="CQ29" s="43"/>
+      <c r="CR29" s="43"/>
+      <c r="CS29" s="43"/>
+      <c r="CT29" s="42"/>
+      <c r="CU29" s="42"/>
+      <c r="CV29" s="42"/>
+      <c r="CW29" s="42"/>
+      <c r="CX29" s="42"/>
+      <c r="CY29" s="42"/>
+      <c r="CZ29" s="42"/>
+      <c r="DA29" s="42"/>
+      <c r="DB29" s="42"/>
+      <c r="DC29" s="42"/>
+      <c r="DD29" s="42"/>
+      <c r="DE29" s="42"/>
+      <c r="DF29" s="42"/>
+      <c r="DG29" s="42"/>
+      <c r="DH29" s="42"/>
+      <c r="DI29" s="42"/>
+      <c r="DJ29" s="42"/>
+      <c r="DK29" s="42"/>
+      <c r="DL29" s="42"/>
+      <c r="DM29" s="42"/>
+      <c r="DN29" s="42"/>
+      <c r="DO29" s="42"/>
+      <c r="DP29" s="42"/>
+      <c r="DQ29" s="42"/>
+      <c r="DR29" s="42"/>
+      <c r="DS29" s="42"/>
+      <c r="DT29" s="42"/>
+      <c r="DU29" s="42"/>
+      <c r="DV29" s="42"/>
+      <c r="DW29" s="42"/>
+      <c r="DX29" s="42"/>
+      <c r="DY29" s="42"/>
+      <c r="DZ29" s="42"/>
+      <c r="EA29" s="42"/>
+      <c r="EB29" s="42"/>
+      <c r="EC29" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="AC2:AK2"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:P4"/>
-    <mergeCell ref="Q4:AK4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:P5"/>
-    <mergeCell ref="H7:V7"/>
-    <mergeCell ref="W7:AK7"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="AL7:AZ7"/>
-    <mergeCell ref="BA7:BO7"/>
-    <mergeCell ref="BP7:CD7"/>
-    <mergeCell ref="CE7:CS7"/>
-    <mergeCell ref="CT7:DH7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AZ8"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="W8:AA8"/>
     <mergeCell ref="CY8:DC8"/>
     <mergeCell ref="DD8:DH8"/>
     <mergeCell ref="B29:BO29"/>
@@ -4807,6 +4978,33 @@
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AG8:AK8"/>
     <mergeCell ref="AL8:AP8"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AZ8"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="W8:AA8"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="AL7:AZ7"/>
+    <mergeCell ref="BA7:BO7"/>
+    <mergeCell ref="BP7:CD7"/>
+    <mergeCell ref="CE7:CS7"/>
+    <mergeCell ref="CT7:DH7"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:P5"/>
+    <mergeCell ref="H7:V7"/>
+    <mergeCell ref="W7:AK7"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="AC2:AK2"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:P4"/>
+    <mergeCell ref="Q4:AK4"/>
   </mergeCells>
   <conditionalFormatting sqref="G20:G27 G15">
     <cfRule type="colorScale" priority="2">

</xml_diff>